<commit_message>
bj: add sch sth forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Benin/2024/bj_sch_sth_impact_202401_1_school_v1.xlsx
+++ b/SCH-STH/Impact assessments/Benin/2024/bj_sch_sth_impact_202401_1_school_v1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TFGH-WHO\Forms\BENIN\SCH STH\Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Benin\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689575AF-4548-4708-99E8-EC37AB0517C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -18,19 +19,6 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913" iterate="1" iterateCount="1000" calcOnSave="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -3225,16 +3213,16 @@
     <t>EPP ZOUZOUVOU</t>
   </si>
   <si>
-    <t>(2024 Janvier) - 1. SCH/STH – Ecole/Localité V1</t>
-  </si>
-  <si>
-    <t>bj_sch_sth_impact_202401_1_school_v1</t>
+    <t>(2024 Janvier) - 1. SCH/STH – Ecole/Localité V2</t>
+  </si>
+  <si>
+    <t>bj_sch_sth_impact_202401_1_school_v2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3877,14 +3865,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1:N1048576"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4915,7 +4903,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G934"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17888,11 +17876,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17930,7 +17918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q174"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>